<commit_message>
Update features by category in biobank.xlsx
</commit_message>
<xml_diff>
--- a/features by category in biobank.xlsx
+++ b/features by category in biobank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adiha\Documents\GitHub\Final-Project-Endo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adiha\Documents\GitHub\ML-Endo-Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DA0C84-AED5-4284-B46E-C61AC0D7F0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0D4901-6EE0-4404-9720-8D512C160570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="348" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>probably male=1 female=0</t>
   </si>
@@ -118,6 +118,117 @@
   </si>
   <si>
     <t>Age at first live birth</t>
+  </si>
+  <si>
+    <t>Currently suffering from problems relating to mood, anxiety and emotions</t>
+  </si>
+  <si>
+    <t>Ever been offered/sought treatment for anxiety</t>
+  </si>
+  <si>
+    <t>Extent affected by problems relating to mood, anxiety and emotions</t>
+  </si>
+  <si>
+    <t>Recent worrying too much about different things</t>
+  </si>
+  <si>
+    <t>Recent trouble relaxing</t>
+  </si>
+  <si>
+    <t>Recent restlessness</t>
+  </si>
+  <si>
+    <t>Recent easy annoyance or irritability</t>
+  </si>
+  <si>
+    <t>Mental health conditions ever diagnosed by a professional</t>
+  </si>
+  <si>
+    <t>Recent feelings or nervousness or anxiety</t>
+  </si>
+  <si>
+    <t>Depression in past six months</t>
+  </si>
+  <si>
+    <t>Depression possibly related to childbirth</t>
+  </si>
+  <si>
+    <t>Ever been offered/sought treatment for depression</t>
+  </si>
+  <si>
+    <t>Seen a psychiatrist for nerves, anxiety, tension or depression</t>
+  </si>
+  <si>
+    <t>Seen doctor (GP) for nerves, anxiety, tension or depression</t>
+  </si>
+  <si>
+    <t>Age at first episode of depression</t>
+  </si>
+  <si>
+    <t>Age at last episode of depression</t>
+  </si>
+  <si>
+    <t>Ever had prolonged feelings of sadness or depression</t>
+  </si>
+  <si>
+    <t>Feelings of tiredness during worst episode of depression</t>
+  </si>
+  <si>
+    <t>Recent feelings of depression</t>
+  </si>
+  <si>
+    <t>Date G43 first reported (migraine)</t>
+  </si>
+  <si>
+    <t>Ever had migraine</t>
+  </si>
+  <si>
+    <t>Date G44 first reported (other headache syndromes)</t>
+  </si>
+  <si>
+    <t>Persistent or recurrent tiredness, weariness or fatigue that has lasted for at least 6 months</t>
+  </si>
+  <si>
+    <t>Recent feelings of tiredness or low energy</t>
+  </si>
+  <si>
+    <t>Currently suffering from mild fatigue</t>
+  </si>
+  <si>
+    <t>Currently suffering from severe fatigue</t>
+  </si>
+  <si>
+    <t>Currently suffering from back pain</t>
+  </si>
+  <si>
+    <t>Hip pain in last three months and rating of pain</t>
+  </si>
+  <si>
+    <t>Back pain in last three months and rating of pain</t>
+  </si>
+  <si>
+    <t>Haemoglobin concentration</t>
+  </si>
+  <si>
+    <t>Haematocrit percentage</t>
+  </si>
+  <si>
+    <t>Red blood cell (erythrocyte) count</t>
+  </si>
+  <si>
+    <t>Oestradiol</t>
+  </si>
+  <si>
+    <t>Date D50 first reported (iron deficiency anaemia)</t>
+  </si>
+  <si>
+    <t>Date D51 first reported (vitamin b12 deficiency anaemia)</t>
+  </si>
+  <si>
+    <t>Date D52 first reported (folate deficiency anaemia)</t>
+  </si>
+  <si>
+    <t>Date D59 first reported (acquired haemolytic anaemia)</t>
   </si>
 </sst>
 </file>
@@ -449,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,9 +573,14 @@
     <col min="6" max="6" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="91.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="44.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="47.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -489,8 +605,32 @@
       <c r="O1" s="2">
         <v>132156</v>
       </c>
+      <c r="R1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="2">
+        <v>28726</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="2">
+        <v>120044</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>131052</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>30020</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -515,8 +655,35 @@
       <c r="O2" s="2">
         <v>132157</v>
       </c>
+      <c r="R2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="2">
+        <v>21062</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="2">
+        <v>20445</v>
+      </c>
+      <c r="X2" s="2">
+        <v>29035</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>120016</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>30030</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -544,8 +711,32 @@
       <c r="O3" s="2">
         <v>132150</v>
       </c>
+      <c r="R3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="2">
+        <v>28728</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="2">
+        <v>21063</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>131054</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>30010</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -570,8 +761,26 @@
       <c r="O4" s="2">
         <v>21050</v>
       </c>
+      <c r="R4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="2">
+        <v>20520</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W4">
+        <v>2100</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>30800</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -596,8 +805,32 @@
       <c r="O5" s="2">
         <v>21026</v>
       </c>
+      <c r="R5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="2">
+        <v>20515</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W5" s="2">
+        <v>2090</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>120114</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>130622</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -622,8 +855,38 @@
       <c r="O6" s="2">
         <v>120017</v>
       </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="2">
+        <v>20516</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="2">
+        <v>20433</v>
+      </c>
+      <c r="X6" s="2">
+        <v>29034</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>20519</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>29005</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>130624</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -648,8 +911,35 @@
       <c r="O7" s="2">
         <v>120043</v>
       </c>
+      <c r="R7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" s="2">
+        <v>20505</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W7" s="2">
+        <v>20434</v>
+      </c>
+      <c r="X7" s="2">
+        <v>29036</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>28696</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>130626</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
@@ -661,6 +951,83 @@
       </c>
       <c r="K8" s="2">
         <v>21047</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="2">
+        <v>29000</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W8" s="2">
+        <v>20446</v>
+      </c>
+      <c r="X8" s="2">
+        <v>29011</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>28699</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>130638</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="R9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" s="2">
+        <v>29058</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W9" s="2">
+        <v>20449</v>
+      </c>
+      <c r="X9" s="2">
+        <v>29018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="V10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="W10" s="2">
+        <v>20510</v>
+      </c>
+      <c r="X10" s="2">
+        <v>29003</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>28639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AA11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>120028</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AA12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>120026</v>
       </c>
     </row>
   </sheetData>
@@ -724,6 +1091,86 @@
     <hyperlink ref="K8" r:id="rId57" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=21047" xr:uid="{7D7D39DB-1A96-442C-AB91-75654AA9E828}"/>
     <hyperlink ref="F8" r:id="rId58" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=2754" xr:uid="{AAEA994F-2BE3-4218-82AE-FBA33B81D7DC}"/>
     <hyperlink ref="G8" r:id="rId59" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=2754" xr:uid="{E60775E9-059A-487D-B06F-808D1AB11D8C}"/>
+    <hyperlink ref="R1" r:id="rId60" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28726" xr:uid="{DC257E30-2C38-4511-B2AC-C1A3CDFD6D4C}"/>
+    <hyperlink ref="S1" r:id="rId61" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28726" xr:uid="{119C3EB6-5B09-4E0E-AA80-7FED469659E2}"/>
+    <hyperlink ref="R2" r:id="rId62" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=21062" xr:uid="{A234AAE3-D443-453B-BB0D-9F88EA50B457}"/>
+    <hyperlink ref="S2" r:id="rId63" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=21062" xr:uid="{63DCBCF6-51A9-44B5-9548-F5B60B7BE122}"/>
+    <hyperlink ref="R3" r:id="rId64" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28728" xr:uid="{DA4871B9-56DB-4B0A-AB4A-8782181BD2F6}"/>
+    <hyperlink ref="S3" r:id="rId65" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28728" xr:uid="{0562B1DC-6C85-4652-90A1-FD9A16598031}"/>
+    <hyperlink ref="R4" r:id="rId66" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20520" xr:uid="{CE78C914-E378-43B8-9BB7-0667AD86000D}"/>
+    <hyperlink ref="S4" r:id="rId67" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20520" xr:uid="{1958FDEC-1014-4D65-9D7D-71D319B66653}"/>
+    <hyperlink ref="R5" r:id="rId68" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20515" xr:uid="{5B90D7F0-A93E-42AF-8EB9-9D6CF3220B27}"/>
+    <hyperlink ref="S5" r:id="rId69" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20515" xr:uid="{C6D33A06-1E2F-4F58-9746-26F83B021563}"/>
+    <hyperlink ref="R6" r:id="rId70" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20516" xr:uid="{082FABBF-9DA4-4BDE-B46B-80C385D8EF82}"/>
+    <hyperlink ref="S6" r:id="rId71" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20516" xr:uid="{C43244E2-7D40-4933-9F60-CD2FF8327863}"/>
+    <hyperlink ref="R7" r:id="rId72" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20505" xr:uid="{AB597911-003E-4E7F-9545-2711AA1ACB71}"/>
+    <hyperlink ref="S7" r:id="rId73" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20505" xr:uid="{C92FCF34-6D8A-49DE-96B7-393FE7EDA54A}"/>
+    <hyperlink ref="R8" r:id="rId74" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29000" xr:uid="{5784F313-6612-4C43-8211-715EB286AE0F}"/>
+    <hyperlink ref="S8" r:id="rId75" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29000" xr:uid="{732439A8-1324-4AC5-8DF8-66B4212C47F5}"/>
+    <hyperlink ref="R9" r:id="rId76" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29058" xr:uid="{E19024DC-9766-4DD3-94EA-60FD173DE5A9}"/>
+    <hyperlink ref="S9" r:id="rId77" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29058" xr:uid="{9C43C032-03C5-45AE-AC31-A40EBD07E1B6}"/>
+    <hyperlink ref="V1" r:id="rId78" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120044" xr:uid="{9BCF48C3-6B38-4B28-9A66-57C8E940D428}"/>
+    <hyperlink ref="W1" r:id="rId79" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120044" xr:uid="{92BABE86-D218-44ED-985F-4B0F264025C9}"/>
+    <hyperlink ref="V2" r:id="rId80" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20445" xr:uid="{863B56EF-787E-47A9-8B27-5BECB52E5E74}"/>
+    <hyperlink ref="W2" r:id="rId81" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20445" xr:uid="{EFAA4F4A-2B19-4E47-9E94-0F11EAC42106}"/>
+    <hyperlink ref="X2" r:id="rId82" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29035" xr:uid="{E4482FA7-3EAF-4AD5-8D16-772D9C405543}"/>
+    <hyperlink ref="V3" r:id="rId83" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=21063" xr:uid="{CF1B0F65-4659-4EA1-A061-85468291762F}"/>
+    <hyperlink ref="W3" r:id="rId84" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=21063" xr:uid="{5255CE1D-CB13-4D43-BB43-8944A90052BA}"/>
+    <hyperlink ref="V4" r:id="rId85" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=2100" xr:uid="{F20B76A5-5B68-4404-9D9E-11F11D910F2B}"/>
+    <hyperlink ref="V5" r:id="rId86" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=2090" xr:uid="{3FC4697A-A8C8-4D5F-8D72-08C03A36D7F7}"/>
+    <hyperlink ref="W5" r:id="rId87" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=2090" xr:uid="{B5861648-59B3-4F12-A9C5-837A11F43D91}"/>
+    <hyperlink ref="V6" r:id="rId88" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20433" xr:uid="{39D3A359-9F74-41E7-99AD-39457D87C08B}"/>
+    <hyperlink ref="W6" r:id="rId89" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20433" xr:uid="{F65A2DE6-D36A-484E-B905-845D466827B1}"/>
+    <hyperlink ref="X6" r:id="rId90" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29034" xr:uid="{BC0220DD-A458-4FE4-9364-62ED3F1CF26D}"/>
+    <hyperlink ref="V7" r:id="rId91" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20434" xr:uid="{BA69209D-68E7-4021-9E0A-AC34DA96EDCD}"/>
+    <hyperlink ref="W7" r:id="rId92" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20434" xr:uid="{B49FDBAB-828C-460D-AE4A-3DC428B14F61}"/>
+    <hyperlink ref="X7" r:id="rId93" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29036" xr:uid="{D8CC54E8-A8D2-4F89-B9C2-7A3D60626D47}"/>
+    <hyperlink ref="V8" r:id="rId94" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20446" xr:uid="{4A605927-1C06-46E5-BB1E-FC5CF8F3ABFF}"/>
+    <hyperlink ref="W8" r:id="rId95" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20446" xr:uid="{5EFA5F7A-C91B-4188-B665-F0168BAF63F6}"/>
+    <hyperlink ref="X8" r:id="rId96" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29011" xr:uid="{8487FD54-1261-435B-AD8D-E9FBEE444E41}"/>
+    <hyperlink ref="V9" r:id="rId97" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20449" xr:uid="{396FB62D-AC0A-4E68-AC27-FF4761DAC0A2}"/>
+    <hyperlink ref="W9" r:id="rId98" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20449" xr:uid="{B83A01B5-B062-46F9-8A89-FDFACD85341E}"/>
+    <hyperlink ref="X9" r:id="rId99" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29018" xr:uid="{5FE91AD5-DE12-4E08-808B-73214C912987}"/>
+    <hyperlink ref="V10" r:id="rId100" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20510" xr:uid="{50AB1FE3-166F-4AC6-8CA1-EB2F6E19B5C2}"/>
+    <hyperlink ref="W10" r:id="rId101" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20510" xr:uid="{DD0681AA-6C39-4397-BA7B-5AEBB6D0C124}"/>
+    <hyperlink ref="X10" r:id="rId102" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29003" xr:uid="{F4B3B781-E3D2-490B-BA5E-82BF32194AE4}"/>
+    <hyperlink ref="AA1" r:id="rId103" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=131052" xr:uid="{140913E0-380A-45BD-AE4D-57D2838D8430}"/>
+    <hyperlink ref="AB1" r:id="rId104" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=131052" xr:uid="{850DC5B7-92DD-45BF-8F9E-C67F4E8C4D76}"/>
+    <hyperlink ref="AA2" r:id="rId105" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120016" xr:uid="{F2AB48CD-E932-4DAA-A83C-B555C72837F1}"/>
+    <hyperlink ref="AB2" r:id="rId106" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120016" xr:uid="{34DDBBF5-9618-4FB6-8D06-0D4B6D5B3C51}"/>
+    <hyperlink ref="AA3" r:id="rId107" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=131054" xr:uid="{C56692FE-D4E9-4AC3-B125-6ED118135BDE}"/>
+    <hyperlink ref="AB3" r:id="rId108" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=131054" xr:uid="{1FC91CAA-A744-44DA-9EBB-0FED79E5F593}"/>
+    <hyperlink ref="AA5" r:id="rId109" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120114" xr:uid="{55678790-3A10-4023-AE5E-1D558DD0379F}"/>
+    <hyperlink ref="AB5" r:id="rId110" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120114" xr:uid="{BEBCBECB-8BFB-4ED7-B23A-8D99805E956B}"/>
+    <hyperlink ref="AA6" r:id="rId111" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20519" xr:uid="{5F00FD39-D270-4718-9E84-1E910FC8A234}"/>
+    <hyperlink ref="AB6" r:id="rId112" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=20519" xr:uid="{397A0FE7-F567-4D53-84DB-D581F8E88070}"/>
+    <hyperlink ref="AC6" r:id="rId113" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=29005" xr:uid="{C5F68E8D-FAE0-43D8-8182-8921088BE750}"/>
+    <hyperlink ref="AA7" r:id="rId114" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28696" xr:uid="{AFA675C3-A058-47B1-836A-C27C478C6EC4}"/>
+    <hyperlink ref="AB7" r:id="rId115" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28696" xr:uid="{EBB3039C-709A-44CC-B3E0-D168C4CD48DF}"/>
+    <hyperlink ref="AA8" r:id="rId116" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28699" xr:uid="{274E6316-FB55-426A-8B1E-3E1830C8C13A}"/>
+    <hyperlink ref="AB8" r:id="rId117" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28699" xr:uid="{29519121-7C4D-4F4A-B448-95273FB54138}"/>
+    <hyperlink ref="AA10" r:id="rId118" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28639" xr:uid="{DA29BBF4-F8F1-43A1-8098-032B1D2FC241}"/>
+    <hyperlink ref="AB10" r:id="rId119" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=28639" xr:uid="{BFEF9E6C-D261-4B49-B4FC-46E2A0761748}"/>
+    <hyperlink ref="AA11" r:id="rId120" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120028" xr:uid="{9797553C-2592-484C-9182-927377B0EDF0}"/>
+    <hyperlink ref="AB11" r:id="rId121" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120028" xr:uid="{DBB6FBCA-402A-4FBE-84F4-01D05F36DB98}"/>
+    <hyperlink ref="AA12" r:id="rId122" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120026" xr:uid="{E2AF47A5-D389-4377-ABBF-B12107018E5D}"/>
+    <hyperlink ref="AB12" r:id="rId123" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=120026" xr:uid="{08175F23-67BA-476B-A27C-881142D4C8B5}"/>
+    <hyperlink ref="AE1" r:id="rId124" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=30020" xr:uid="{5FB57860-D977-400F-B559-5176EA3367A8}"/>
+    <hyperlink ref="AF1" r:id="rId125" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=30020" xr:uid="{86E922C6-89CB-4A8D-9C58-9AB9A1293F75}"/>
+    <hyperlink ref="AE2" r:id="rId126" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=30030" xr:uid="{47898A1D-E5F2-4853-B83E-28F953B839EA}"/>
+    <hyperlink ref="AF2" r:id="rId127" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=30030" xr:uid="{ACA03363-7207-4108-9DC1-88856B00CE3E}"/>
+    <hyperlink ref="AE3" r:id="rId128" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=30010" xr:uid="{467EB25D-E396-4538-AB00-6CBEB0330A90}"/>
+    <hyperlink ref="AF3" r:id="rId129" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=30010" xr:uid="{6D00317C-0361-41B0-95FA-675E399132A3}"/>
+    <hyperlink ref="AE4" r:id="rId130" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=30800" xr:uid="{5893A843-00D7-426C-B717-BA6A33E7863F}"/>
+    <hyperlink ref="AF4" r:id="rId131" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=30800" xr:uid="{B2CA50B1-6057-4D02-98D9-1CB5989EFC01}"/>
+    <hyperlink ref="AE5" r:id="rId132" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=130622" xr:uid="{5CEC155A-F649-4326-9707-C8D4545B9AB7}"/>
+    <hyperlink ref="AF5" r:id="rId133" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=130622" xr:uid="{85ACD6B6-EC1C-47A5-BF16-3317DA3B57EC}"/>
+    <hyperlink ref="AE6" r:id="rId134" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=130624" xr:uid="{C7F38147-88F9-4D10-8780-7ACF8863B7D3}"/>
+    <hyperlink ref="AF6" r:id="rId135" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=130624" xr:uid="{7D58981F-92C9-4DCE-BEC6-446CC06DB0CE}"/>
+    <hyperlink ref="AE7" r:id="rId136" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=130626" xr:uid="{3B436D18-0201-435D-A130-9842D5EC52F7}"/>
+    <hyperlink ref="AF7" r:id="rId137" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=130626" xr:uid="{2699C95C-1F41-4B14-9A0B-1B5DD797DE00}"/>
+    <hyperlink ref="AE8" r:id="rId138" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=130638" xr:uid="{C1F69BB1-DFF8-4ED4-9201-DBF5B9267ED8}"/>
+    <hyperlink ref="AF8" r:id="rId139" display="https://biobank.ndph.ox.ac.uk/showcase/field.cgi?id=130638" xr:uid="{9CCAC264-F0E7-404C-B415-C7BD9C7D1F9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to project summary and presentation
</commit_message>
<xml_diff>
--- a/features by category in biobank.xlsx
+++ b/features by category in biobank.xlsx
@@ -1,32 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adiha\Documents\GitHub\ML-Endo-Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B17060-29D6-4100-88BD-6011E5496C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E3197F-D7E6-47B4-BD61-F1A8A0A4DF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet3!$A$1:$A$7</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet3!$B$1:$B$7</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet3!$A$1:$A$7</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet3!$B$1:$B$7</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Sheet3!$A$1:$A$7</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Sheet3!$B$1:$B$7</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Sheet3!$A$1:$A$7</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Sheet3!$B$1:$B$7</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="119">
   <si>
     <t>probably male=1 female=0</t>
   </si>
@@ -362,6 +384,27 @@
   </si>
   <si>
     <t>Vitamin E</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Pain indicators</t>
+  </si>
+  <si>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>Menstruation</t>
+  </si>
+  <si>
+    <t>Mental health</t>
+  </si>
+  <si>
+    <t>Related illnesses</t>
+  </si>
+  <si>
+    <t>infertility</t>
   </si>
 </sst>
 </file>
@@ -437,10 +480,1695 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Features by Subject</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32512454811073144"/>
+          <c:y val="0.15312777585402204"/>
+          <c:w val="0.33088322686079336"/>
+          <c:h val="0.5029678113849535"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-IL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$1:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>General</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pain indicators</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>infertility</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Diet</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Menstruation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mental health</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Related illnesses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$1:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7314-4FC7-A892-4367680DE8F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="55"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13929618768328444"/>
+          <c:y val="0.67375604101112596"/>
+          <c:w val="0.67573256055603015"/>
+          <c:h val="0.27366269703858714"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v2.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v2.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Features by Subject</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IL" sz="1400">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="funnel" uniqueId="{615B9932-C2B1-4B8B-9B94-B6B47AE04965}">
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="1">
+        <cx:catScaling gapWidth="0.0599999987"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="419">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314960</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55AF8E90-5BBA-761C-1A75-F73005862AB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78BC7833-CD39-9EC3-6B34-530A914D45A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2956560" y="4339590"/>
+              <a:ext cx="4785360" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-IL" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Custom 1">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -457,16 +2185,16 @@
         <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="FF99CC"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="954F72"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="DB92F2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="47C1B0"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -702,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AI4" sqref="AI4"/>
+    <sheetView topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1625,7 +3353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29356CCF-2910-4F95-85DD-48185113FA8A}">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A95" workbookViewId="0">
       <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
@@ -2647,4 +4375,86 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334E8625-333A-406B-939F-407C45FCBFE1}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <f>SUM(B1:B7)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>